<commit_message>
template download according to add,delete
</commit_message>
<xml_diff>
--- a/external/uploads/endorsement_export.xlsx
+++ b/external/uploads/endorsement_export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Corporate</t>
   </si>
@@ -23,22 +23,40 @@
     <t>employee</t>
   </si>
   <si>
+    <t>age</t>
+  </si>
+  <si>
     <t>sum insured</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>2002-01-23</t>
+    <t>A- AdditionD - DeletionC -Change</t>
+  </si>
+  <si>
+    <t>Date of joining</t>
+  </si>
+  <si>
+    <t>Date of Leaving</t>
   </si>
   <si>
     <t>Demo Account</t>
   </si>
   <si>
+    <t>Abdul Quadir</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>01-01-1970</t>
+  </si>
+  <si>
+    <t>29-03-2023</t>
+  </si>
+  <si>
     <t>Avinash</t>
   </si>
   <si>
-    <t>New Addition</t>
+    <t>A</t>
   </si>
   <si>
     <t>12-03-2023</t>
@@ -63,12 +81,12 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -81,7 +99,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
+        <fgColor rgb="FF0000ff"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -398,58 +416,82 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>45</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>200000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>300000</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rules and template done
</commit_message>
<xml_diff>
--- a/external/uploads/endorsement_export.xlsx
+++ b/external/uploads/endorsement_export.xlsx
@@ -15,68 +15,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
-  <si>
-    <t>S_No</t>
-  </si>
-  <si>
-    <t>Policy_No</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Employee code</t>
-  </si>
-  <si>
-    <t>Insured_Name</t>
-  </si>
-  <si>
-    <t>Relationship_type</t>
-  </si>
-  <si>
-    <t>Date_of_Birth</t>
-  </si>
-  <si>
-    <t>Sum_Insured</t>
-  </si>
-  <si>
-    <t>Date_of_Joining</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>Date_of_Marriage</t>
-  </si>
-  <si>
-    <t>Remarks_for_Corrections</t>
-  </si>
-  <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
-  </si>
-  <si>
-    <t>Mobile_No</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>Policy Number</t>
+  </si>
+  <si>
+    <t>Member Name</t>
+  </si>
+  <si>
+    <t>Sum Insured</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Endorsement_Effective_Date</t>
-  </si>
-  <si>
-    <t>Premium_including_GST</t>
-  </si>
-  <si>
-    <t>Wrong_DETAILS</t>
-  </si>
-  <si>
     <t>2215041121P102938067</t>
   </si>
   <si>
+    <t>Deletion</t>
+  </si>
+  <si>
     <t>1003RB</t>
   </si>
   <si>
@@ -92,25 +50,13 @@
     <t>01-01-1970</t>
   </si>
   <si>
+    <t>29-03-2023</t>
+  </si>
+  <si>
     <t>Abdul Quadir</t>
   </si>
   <si>
     <t>null</t>
-  </si>
-  <si>
-    <t>1006RB</t>
-  </si>
-  <si>
-    <t>25-04-1994</t>
-  </si>
-  <si>
-    <t>12-03-2023</t>
-  </si>
-  <si>
-    <t>Avinash</t>
-  </si>
-  <si>
-    <t>admin@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -464,7 +410,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="U1" sqref="U1"/>
@@ -472,26 +418,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="4" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="4" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="3" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="15" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="31" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="3" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="4" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="8" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -508,79 +454,45 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>39</v>
@@ -589,31 +501,31 @@
         <v>200000</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2">
-        <v>200000</v>
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O2">
         <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="S2">
         <v>400.0</v>
@@ -623,71 +535,6 @@
       </c>
       <c r="U2">
         <v>200000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3">
-        <v>28</v>
-      </c>
-      <c r="I3">
-        <v>300000</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3">
-        <v>300000</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3">
-        <v>28</v>
-      </c>
-      <c r="P3">
-        <v>9999999999</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3">
-        <v>400.0</v>
-      </c>
-      <c r="T3">
-        <v>300000</v>
-      </c>
-      <c r="U3">
-        <v>300000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>